<commit_message>
Fixed typo and formatting
</commit_message>
<xml_diff>
--- a/labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
+++ b/labs/Lab02/CS133JS_Lab02_Rubrics.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/labs/Lab02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA440639-C772-3E4B-B57B-5939C198735E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5943263F-1AA5-4441-9492-300B8BBAC443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="2220" windowWidth="25600" windowHeight="14520" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="32760" yWindow="4896" windowWidth="15744" windowHeight="11208" activeTab="2" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
     <sheet name="Group B" sheetId="4" r:id="rId2"/>
     <sheet name="Group C" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -44,9 +54,6 @@
     <t>Part 1</t>
   </si>
   <si>
-    <t>Function exercises in the concole</t>
-  </si>
-  <si>
     <t>Part 2</t>
   </si>
   <si>
@@ -93,13 +100,16 @@
   </si>
   <si>
     <t>Cost per mile app functionality</t>
+  </si>
+  <si>
+    <t>Function exercises in the console</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,11 +132,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,8 +158,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,24 +476,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,34 +504,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -535,9 +540,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -546,9 +551,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -557,9 +562,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
@@ -568,9 +573,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -579,9 +584,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -590,9 +595,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -601,9 +606,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -612,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -627,6 +632,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -635,23 +641,23 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -662,34 +668,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -698,9 +704,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -709,9 +715,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -720,9 +726,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
@@ -731,9 +737,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -742,9 +748,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -753,9 +759,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -764,9 +770,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -775,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -787,8 +793,8 @@
         <f>SUM(E5:E14)</f>
         <v>50</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>14</v>
+      <c r="F16" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -800,24 +806,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F5606A-302D-8F40-B769-19B85F064B34}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -828,34 +834,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -864,9 +870,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -875,9 +881,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -886,9 +892,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
@@ -897,9 +903,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -908,9 +914,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -919,9 +925,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -930,9 +936,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -941,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -953,8 +959,8 @@
         <f>SUM(E5:E14)</f>
         <v>50</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>14</v>
+      <c r="F16" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>